<commit_message>
Getting messages was done
This was complicated. Some of you might want to expect a merge error.

@lucabesana97
@MihaiNico
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626A7D7D-F0DC-428C-985B-2D016D560095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2649DEDA-A8FB-4849-94E2-F6FF58359595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2508" yWindow="2172" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Time Log </t>
   </si>
@@ -90,7 +90,10 @@
     <t xml:space="preserve">Set up the Database server on the server we got from the CS department. Had a development meeting with Luca and Mihai. Assisted most of the team with getting connected to A. The database server, B. the Github repository, or C. Both. Task  16: Created the methods necessary to post a message but did not implement the business logic within those methods. Added documentation to methods to better connect to the front-end. Task 6: Wrapped SPROC inside a transaction. No parameters actually needed to be validated since they are all OUT parameters. Fixed the bug that had the session ID always be 2 if the session did not exist. </t>
   </si>
   <si>
-    <t>Task 22: Got some basic error checking working. Can catch the exceptions though right now they're just ignored. Task 13: Taught Shammi how to make a Stored Procedure, Throw Errors, Do IF statements, and store variables in tSQL. Task 17: Created the SPROC to insert a reply into the database</t>
+    <t>Task 22: Got some basic error checking working. Can catch the exceptions though right now they're just ignored. Task 13: Taught Shammi how to make a Stored Procedure, Throw Errors, Do IF statements, and store variables in tSQL. Task 17: Created the SPROC to insert a reply into the database.</t>
+  </si>
+  <si>
+    <t>Task 16: Complete.</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -730,8 +733,12 @@
         <f t="shared" si="1"/>
         <v>44157</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="E14" s="12">
+        <v>2</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11">

</xml_diff>

<commit_message>
Worked on JUnit tests
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2649DEDA-A8FB-4849-94E2-F6FF58359595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F143602A-2FAF-48CD-959E-A6EA7489E9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2508" yWindow="2172" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
     <t>Task 22: Got some basic error checking working. Can catch the exceptions though right now they're just ignored. Task 13: Taught Shammi how to make a Stored Procedure, Throw Errors, Do IF statements, and store variables in tSQL. Task 17: Created the SPROC to insert a reply into the database.</t>
   </si>
   <si>
-    <t>Task 16: Complete.</t>
+    <t>Task 16: Complete. Task 18: Complete</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -734,7 +734,7 @@
         <v>44157</v>
       </c>
       <c r="E14" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Work on JUnit tests
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F143602A-2FAF-48CD-959E-A6EA7489E9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4A182B-A1AC-4BF8-BB27-43ED792A4BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2508" yWindow="2172" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
     <t>Task 22: Got some basic error checking working. Can catch the exceptions though right now they're just ignored. Task 13: Taught Shammi how to make a Stored Procedure, Throw Errors, Do IF statements, and store variables in tSQL. Task 17: Created the SPROC to insert a reply into the database.</t>
   </si>
   <si>
-    <t>Task 16: Complete. Task 18: Complete</t>
+    <t>Task 16: Complete. Task 18: Complete. Task 27: Preliminary work. Could never get it working. 30 minute meeting with Luca to resolve a merge conflict.</t>
   </si>
 </sst>
 </file>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -734,7 +734,7 @@
         <v>44157</v>
       </c>
       <c r="E14" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
More work on JUNIT tests
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4A182B-A1AC-4BF8-BB27-43ED792A4BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDEBBFD-9207-4832-AA54-4F123B9D95F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2508" yWindow="2172" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
     <t>Task 22: Got some basic error checking working. Can catch the exceptions though right now they're just ignored. Task 13: Taught Shammi how to make a Stored Procedure, Throw Errors, Do IF statements, and store variables in tSQL. Task 17: Created the SPROC to insert a reply into the database.</t>
   </si>
   <si>
-    <t>Task 16: Complete. Task 18: Complete. Task 27: Preliminary work. Could never get it working. 30 minute meeting with Luca to resolve a merge conflict.</t>
+    <t>Task 16: Complete. Task 18: Complete. Task 27: Created testing for creatingSessions. 30 minute meeting with Luca to resolve a merge conflict.</t>
   </si>
 </sst>
 </file>
@@ -734,7 +734,7 @@
         <v>44157</v>
       </c>
       <c r="E14" s="12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Join Real Session JUNIT test done
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDEBBFD-9207-4832-AA54-4F123B9D95F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66633315-04AB-4550-BAF8-75BA0F6C96C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2508" yWindow="2172" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -499,7 +499,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -734,7 +734,7 @@
         <v>44157</v>
       </c>
       <c r="E14" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Fixed that annoying bug I talked about at SCRUM
Objects no longer infinitely loop.
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hs-ulm.de\fs\users\pepeco01\Eigene Dateien\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01F8191-A9F0-4719-828B-47934BB2A0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="500"/>
+    <workbookView xWindow="2508" yWindow="2172" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Time Log </t>
   </si>
@@ -96,12 +97,15 @@
   </si>
   <si>
     <t>Task 4 &amp; 6: Completed backend and database implementation of message updating. Task 16: Laid out the groundwork for updating. Downloaded all necessary software to develop stuff without my own computer. All of this is on the Server. Reformatted some code to a different response body we might want to use. Not being used yet. Task 16: Complete. Task 26: Complete</t>
+  </si>
+  <si>
+    <t>Added missing model classes into backend application. Fixed infinite looping object problem.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -227,7 +231,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -504,22 +508,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="5" customWidth="1"/>
-    <col min="2" max="4" width="11.25" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.25" style="13"/>
-    <col min="6" max="6" width="151.25" customWidth="1"/>
+    <col min="2" max="4" width="11.19921875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.19921875" style="13"/>
+    <col min="6" max="6" width="151.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -529,7 +533,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
       <c r="E3" s="14" t="s">
         <v>1</v>
@@ -538,7 +542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
       <c r="E4" s="14" t="s">
         <v>2</v>
@@ -547,7 +551,7 @@
         <v>6003129</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
@@ -567,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>1</v>
       </c>
@@ -589,7 +593,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>2</v>
       </c>
@@ -612,7 +616,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>3</v>
       </c>
@@ -635,7 +639,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>4</v>
       </c>
@@ -658,7 +662,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>5</v>
       </c>
@@ -681,7 +685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>6</v>
       </c>
@@ -704,7 +708,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>7</v>
       </c>
@@ -727,7 +731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>8</v>
       </c>
@@ -750,7 +754,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>9</v>
       </c>
@@ -773,7 +777,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>10</v>
       </c>
@@ -789,10 +793,14 @@
         <f t="shared" si="1"/>
         <v>44171</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>11</v>
       </c>
@@ -811,7 +819,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>12</v>
       </c>
@@ -830,7 +838,7 @@
       <c r="E18" s="16"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>13</v>
       </c>
@@ -849,7 +857,7 @@
       <c r="E19" s="16"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>14</v>
       </c>
@@ -868,7 +876,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>15</v>
       </c>
@@ -887,7 +895,7 @@
       <c r="E21" s="16"/>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Revert "JUnit tests work"
This reverts commit c7913619a1d9dd9d4a2f45a313bf8accf877f1b1.
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0B712C-1BDB-4CFE-8092-74611F908E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6FBC21-C095-479E-9D25-3AE963D6156A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2568" yWindow="1416" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -794,7 +794,7 @@
         <v>44171</v>
       </c>
       <c r="E16" s="16">
-        <v>6.7</v>
+        <v>5.2</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Revert "Revert "JUnit tests work""
This reverts commit 38c0ada0f358e457981cba35f938e389f1221b4c.
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6FBC21-C095-479E-9D25-3AE963D6156A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0B712C-1BDB-4CFE-8092-74611F908E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2568" yWindow="1416" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -794,7 +794,7 @@
         <v>44171</v>
       </c>
       <c r="E16" s="16">
-        <v>5.2</v>
+        <v>6.7</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/leafcathead/CTS5_AudienceResponse"
This reverts commit 2729a805f12c773875cc146f287299cbde6dbcf1, reversing
changes made to 03b035430098215e004df6c65db7868fd874cdfa.
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06B1ED1-D1A2-4CFA-B586-5CE3791FEA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6FBC21-C095-479E-9D25-3AE963D6156A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="1560" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2568" yWindow="1416" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Time Log </t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Added missing model classes into backend application. Fixed infinite looping object problem. Fixed JS to correctly get stuff out of a map. Task 5: Fixed a bug involving POJOs, got the connection to the controller finished. Task 5: Completed. Had to revamp DELETE_MESSAGE to delete everything as it should. Task 28: Worked on Junit tests.</t>
-  </si>
-  <si>
-    <t>Created CLOSE_SESSION SPROC for next Sprint</t>
   </si>
 </sst>
 </file>
@@ -515,7 +512,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -797,7 +794,7 @@
         <v>44171</v>
       </c>
       <c r="E16" s="16">
-        <v>7</v>
+        <v>5.2</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>20</v>
@@ -819,12 +816,8 @@
         <f t="shared" si="1"/>
         <v>44178</v>
       </c>
-      <c r="E17" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>21</v>
-      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">

</xml_diff>

<commit_message>
Worked on Message Likes
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6FBC21-C095-479E-9D25-3AE963D6156A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33629A56-D6BC-428E-9949-72E734985D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2568" yWindow="1416" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="1560" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Time Log </t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Added missing model classes into backend application. Fixed infinite looping object problem. Fixed JS to correctly get stuff out of a map. Task 5: Fixed a bug involving POJOs, got the connection to the controller finished. Task 5: Completed. Had to revamp DELETE_MESSAGE to delete everything as it should. Task 28: Worked on Junit tests.</t>
+  </si>
+  <si>
+    <t>I had stuff here but people recklessly reverted commits and then commited those reverts to the head branch. They did so without telling anyone and now I cannot figure out what I did specifically or what is missing from the application!</t>
+  </si>
+  <si>
+    <t>Added new "Likes" table wrote backend code to update likes in the database.</t>
   </si>
 </sst>
 </file>
@@ -512,7 +518,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -794,7 +800,7 @@
         <v>44171</v>
       </c>
       <c r="E16" s="16">
-        <v>5.2</v>
+        <v>7</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>20</v>
@@ -816,8 +822,12 @@
         <f t="shared" si="1"/>
         <v>44178</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="11"/>
+      <c r="E17" s="16">
+        <v>3</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
@@ -835,8 +845,12 @@
         <f t="shared" si="1"/>
         <v>44185</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="11"/>
+      <c r="E18" s="16">
+        <v>1</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="19" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10">

</xml_diff>

<commit_message>
Worked on session closing
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33629A56-D6BC-428E-9949-72E734985D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4DB35A-2FAC-46C1-AC7B-B0503FD62BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="1560" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,7 +105,7 @@
     <t>I had stuff here but people recklessly reverted commits and then commited those reverts to the head branch. They did so without telling anyone and now I cannot figure out what I did specifically or what is missing from the application!</t>
   </si>
   <si>
-    <t>Added new "Likes" table wrote backend code to update likes in the database.</t>
+    <t>Added new "Likes" table wrote backend code to update likes in the database. Added backend code to close a session. Not tested. Have not been able to connect to VPN even on campus.</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -846,7 +846,7 @@
         <v>44185</v>
       </c>
       <c r="E18" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Bug fixes, likes now working
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4DB35A-2FAC-46C1-AC7B-B0503FD62BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF93934C-F2B6-484B-8549-FAD05B421A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="1560" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,7 +105,7 @@
     <t>I had stuff here but people recklessly reverted commits and then commited those reverts to the head branch. They did so without telling anyone and now I cannot figure out what I did specifically or what is missing from the application!</t>
   </si>
   <si>
-    <t>Added new "Likes" table wrote backend code to update likes in the database. Added backend code to close a session. Not tested. Have not been able to connect to VPN even on campus.</t>
+    <t>Added new "Likes" table wrote backend code to update likes in the database. Added backend code to close a session.. Fixed bugs in deleting message and fixed bugs in Junit tests involving the test to update message content and the test to delete messages. Fixed a JUnit test bug where we were testing the wrong procedure. Wrote SPROC to toggle likes on a message</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -846,7 +846,7 @@
         <v>44185</v>
       </c>
       <c r="E18" s="16">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Added Junit tests for messages. Fixed a few error checking bugs.
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F0EAC2-F281-4FFC-BFA5-2EAFFA5651AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFE6AEF-6FFB-42C1-9228-0451C1DBF858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="1560" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,7 +105,7 @@
     <t>I had stuff here but people recklessly reverted commits and then commited those reverts to the head branch. They did so without telling anyone and now I cannot figure out what I did specifically or what is missing from the application!</t>
   </si>
   <si>
-    <t>Added new "Likes" table wrote backend code to update likes in the database. Added backend code to close a session.. Fixed bugs in deleting message and fixed bugs in Junit tests involving the test to update message content and the test to delete messages. Fixed a JUnit test bug where we were testing the wrong procedure. Wrote SPROC to toggle likes on a message. Complete close session</t>
+    <t>Added new "Likes" table wrote backend code to update likes in the database. Added backend code to close a session.. Fixed bugs in deleting message and fixed bugs in Junit tests involving the test to update message content and the test to delete messages. Fixed a JUnit test bug where we were testing the wrong procedure. Wrote SPROC to toggle likes on a message. Complete close session. Wrote new Junit tests for bad delete requests.</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -846,7 +846,7 @@
         <v>44185</v>
       </c>
       <c r="E18" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Updated close sessions tests and fixed bug in closing session
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0964F0C2-9E32-431B-87C8-8378C37B38A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EEFECD-E46A-48A1-B1B5-0B01F57D31E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="1560" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4368" yWindow="1908" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Time Log </t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Finished last few API calls. Deleted unused code.</t>
+  </si>
+  <si>
+    <t>Finalized sesssion closing. Bug fixes. Cleaned up unused code. Added some documentation. Migrated to a different Stored Procedure to close sessions, changed tests accordingly.</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -946,8 +949,12 @@
         <f t="shared" si="1"/>
         <v>44213</v>
       </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="11"/>
+      <c r="E22" s="16">
+        <v>6</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created a cleaner implementation for "checkSessionStatus"
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EEFECD-E46A-48A1-B1B5-0B01F57D31E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D640FCA3-BDE5-4BB4-BA1E-6E4026D52E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4368" yWindow="1908" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,7 +117,7 @@
     <t>Finished last few API calls. Deleted unused code.</t>
   </si>
   <si>
-    <t>Finalized sesssion closing. Bug fixes. Cleaned up unused code. Added some documentation. Migrated to a different Stored Procedure to close sessions, changed tests accordingly.</t>
+    <t>Finalized sesssion closing. Bug fixes. Cleaned up unused code. Added some documentation. Migrated to a different Stored Procedure to close sessions, changed tests accordingly. Re-wrote inserting panic responses since Luca and Mihai obviously never tested it.</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated Session tests to reflect HTTPS
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11C34C0-DE78-4D97-95A0-E77D675BDDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C061F838-45CA-4263-A604-439D957CC7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="1560" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,7 +117,7 @@
     <t>Finished last few API calls. Deleted unused code.</t>
   </si>
   <si>
-    <t>Finalized sesssion closing. Bug fixes. Cleaned up unused code. Added some documentation. Migrated to a different Stored Procedure to close sessions, changed tests accordingly. Re-wrote inserting panic responses since Luca and Mihai obviously never tested it. Finally completed web sockets!</t>
+    <t>Finalized sesssion closing. Bug fixes. Cleaned up unused code. Added some documentation. Migrated to a different Stored Procedure to close sessions, changed tests accordingly. Re-wrote inserting panic responses since Luca and Mihai obviously never tested it. Finally completed web sockets! Finished HTTPS</t>
   </si>
 </sst>
 </file>
@@ -950,7 +950,7 @@
         <v>44213</v>
       </c>
       <c r="E22" s="16">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Changes to API calls and async behavior
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
+++ b/Documentation/SCRUM/TimeLog_ConnorPeper.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pepercr\Documents\Rose-Local\Software Project\AudienceResponse\CTS5_AudienceResponse\Documentation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C061F838-45CA-4263-A604-439D957CC7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464C8C64-8636-4777-8359-F5EB3865191C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="1560" windowWidth="17472" windowHeight="9876" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,7 +117,7 @@
     <t>Finished last few API calls. Deleted unused code.</t>
   </si>
   <si>
-    <t>Finalized sesssion closing. Bug fixes. Cleaned up unused code. Added some documentation. Migrated to a different Stored Procedure to close sessions, changed tests accordingly. Re-wrote inserting panic responses since Luca and Mihai obviously never tested it. Finally completed web sockets! Finished HTTPS</t>
+    <t>Finalized sesssion closing. Bug fixes. Cleaned up unused code. Added some documentation. Migrated to a different Stored Procedure to close sessions, changed tests accordingly. Re-wrote inserting panic responses since Luca and Mihai obviously never tested it. Finally completed web sockets! Finished HTTPS. Hosted the Spring Boot server on the remote server. Fixed bugs and re-did the architecture notebook and updated all diagrams to reflect the release state of the application.</t>
   </si>
 </sst>
 </file>
@@ -530,7 +530,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -950,7 +950,7 @@
         <v>44213</v>
       </c>
       <c r="E22" s="16">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>26</v>

</xml_diff>